<commit_message>
Update test for spreadsheet type
</commit_message>
<xml_diff>
--- a/atomica/library/framework_template.xlsx
+++ b/atomica/library/framework_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAC4E37-BDD0-4F1C-A699-CF85B498DE87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147C9689-62D8-4514-917D-80A656643475}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1472,26 +1472,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="About"/>
       <sheetName val="Databook Pages"/>
-      <sheetName val="Compartments"/>
-      <sheetName val="Transitions"/>
-      <sheetName val="Characteristics"/>
-      <sheetName val="Parameters"/>
-      <sheetName val="Interactions"/>
-      <sheetName val="Cascades"/>
-      <sheetName val="Plots"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>